<commit_message>
working on the main method- classes are done wiating to be tested
</commit_message>
<xml_diff>
--- a/SA/resources/GuestList.xlsx
+++ b/SA/resources/GuestList.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osofri\Desktop\git projects\java_project\SA\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F89C24-85A5-47E0-A2C4-7AE8514A346C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860530F9-8A2A-48DF-96EF-33F17A788B67}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{943ECB27-B148-4AFB-9FF3-42F2DC5793B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GuestList" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Full name</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Nava Boker</t>
+  </si>
+  <si>
+    <t>nisayon ert</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +543,15 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>

</xml_diff>

<commit_message>
fixed some bugs in Node class and added functions to Main class
</commit_message>
<xml_diff>
--- a/SA/resources/GuestList.xlsx
+++ b/SA/resources/GuestList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osofri\Desktop\git projects\java_project\SA\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860530F9-8A2A-48DF-96EF-33F17A788B67}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC377805-6257-4819-81AC-2AEEA66D4C4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{943ECB27-B148-4AFB-9FF3-42F2DC5793B6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Full name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>nisayon ert</t>
+  </si>
+  <si>
+    <t>takale letikun</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>